<commit_message>
starting to delve into p1/2 problems, sperated curve stripping fucntion for each phase[in operations.py])
</commit_message>
<xml_diff>
--- a/CATE Template - Single Run.xlsx
+++ b/CATE Template - Single Run.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Vial #</t>
   </si>
   <si>
     <t>Elution time (min)</t>
-  </si>
-  <si>
-    <t>Activity in eluant (cpm)</t>
   </si>
   <si>
     <t>Specific Activity (cpm · µmol⁻¹)</t>
@@ -40,17 +37,17 @@
     <t>G-Factor</t>
   </si>
   <si>
-    <t>Run 1</t>
+    <t>Load Time (min)</t>
   </si>
   <si>
-    <t>Load Time (min)</t>
+    <t>Run5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +72,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -126,11 +127,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -144,19 +146,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,72 +464,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11">
+        <v>7141.4219999999996</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="9">
-        <v>35714.844999999994</v>
-      </c>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="12">
+        <v>5170.1000000000004</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="10">
-        <v>8679.2999999999993</v>
-      </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="12">
+        <v>1712</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="10">
-        <v>4746.2</v>
-      </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="13">
+        <v>0.36049999999999915</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="11">
-        <v>0.60270000000000046</v>
-      </c>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="14">
+        <v>1.0245470760959214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6">
-        <v>1.0084176343828561</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="4">
         <v>60</v>
       </c>
@@ -535,339 +542,336 @@
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="6">
-        <v>81453</v>
+      <c r="C9" s="15">
+        <v>52437</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="6">
-        <v>20369.099999999999</v>
+      <c r="C10" s="15">
+        <v>9144.4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>3</v>
       </c>
-      <c r="C11" s="6">
-        <v>5511</v>
+      <c r="C11" s="15">
+        <v>2880.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>4</v>
       </c>
-      <c r="C12" s="6">
-        <v>2790.7</v>
+      <c r="C12" s="15">
+        <v>1585.1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="6">
-        <v>1933.8</v>
+      <c r="C13" s="15">
+        <v>1156.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="6">
-        <v>1456.8</v>
+      <c r="C14" s="15">
+        <v>923.4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>7</v>
       </c>
-      <c r="C15" s="6">
-        <v>1159.5</v>
+      <c r="C15" s="15">
+        <v>788.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>8</v>
       </c>
-      <c r="C16" s="6">
-        <v>1015.1</v>
+      <c r="C16" s="15">
+        <v>720.7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>9</v>
       </c>
-      <c r="C17" s="6">
-        <v>882.4</v>
+      <c r="C17" s="15">
+        <v>764.2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>10</v>
       </c>
-      <c r="C18" s="6">
-        <v>788.5</v>
+      <c r="C18" s="15">
+        <v>649</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>11.5</v>
       </c>
-      <c r="C19" s="6">
-        <v>801.7</v>
+      <c r="C19" s="15">
+        <v>644.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>13</v>
       </c>
-      <c r="C20" s="6">
-        <v>698.5</v>
+      <c r="C20" s="15">
+        <v>738.4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>14.5</v>
       </c>
-      <c r="C21" s="6">
-        <v>647.9</v>
+      <c r="C21" s="15">
+        <v>549.79999999999995</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>16</v>
       </c>
-      <c r="C22" s="6">
-        <v>629.29999999999995</v>
+      <c r="C22" s="15">
+        <v>522</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>17.5</v>
       </c>
-      <c r="C23" s="6">
-        <v>622.20000000000005</v>
+      <c r="C23" s="15">
+        <v>544</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>19</v>
       </c>
-      <c r="C24" s="6">
-        <v>507.9</v>
+      <c r="C24" s="15">
+        <v>496.6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>20.5</v>
       </c>
-      <c r="C25" s="6">
-        <v>504.2</v>
+      <c r="C25" s="15">
+        <v>438.6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>22</v>
       </c>
-      <c r="C26" s="6">
-        <v>422.8</v>
+      <c r="C26" s="15">
+        <v>352.3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>23.5</v>
       </c>
-      <c r="C27" s="6">
-        <v>451.9</v>
+      <c r="C27" s="15">
+        <v>392.9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="5">
         <v>25</v>
       </c>
-      <c r="C28" s="6">
-        <v>411.3</v>
+      <c r="C28" s="15">
+        <v>297.89999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>27</v>
       </c>
-      <c r="C29" s="6">
-        <v>475.7</v>
+      <c r="C29" s="15">
+        <v>472.1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="5">
         <v>29</v>
       </c>
-      <c r="C30" s="6">
-        <v>453.3</v>
+      <c r="C30" s="15">
+        <v>382.1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="5">
         <v>31</v>
       </c>
-      <c r="C31" s="6">
-        <v>467.4</v>
+      <c r="C31" s="15">
+        <v>412.9</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>24</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="5">
         <v>33</v>
       </c>
-      <c r="C32" s="6">
-        <v>431.2</v>
+      <c r="C32" s="15">
+        <v>399.8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="5">
         <v>35</v>
       </c>
-      <c r="C33" s="6">
-        <v>404.4</v>
+      <c r="C33" s="15">
+        <v>322.8</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="5">
         <v>37</v>
       </c>
-      <c r="C34" s="6">
-        <v>432.2</v>
+      <c r="C34" s="15">
+        <v>375.2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>27</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="5">
         <v>39</v>
       </c>
-      <c r="C35" s="6">
-        <v>363.8</v>
+      <c r="C35" s="15">
+        <v>342.1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="5">
         <v>41</v>
       </c>
-      <c r="C36" s="6">
-        <v>429.8</v>
+      <c r="C36" s="15">
+        <v>387.8</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="5">
         <v>43</v>
       </c>
-      <c r="C37" s="6">
-        <v>303.39999999999998</v>
+      <c r="C37" s="15">
+        <v>303.89999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="5">
         <v>45</v>
       </c>
-      <c r="C38" s="6">
-        <v>348.1</v>
+      <c r="C38" s="15">
+        <v>324.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
playing with row alignment in excel summary sheet. starting output of phase corrected data. may require unifying sbj/obj analysis objects
</commit_message>
<xml_diff>
--- a/CATE Template - Single Run.xlsx
+++ b/CATE Template - Single Run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" calcOnSave="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -98,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -126,13 +126,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -151,14 +160,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,59 +487,59 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11">
-        <v>7141.4219999999996</v>
+      <c r="B2" s="12"/>
+      <c r="C2">
+        <v>7180.7628571428577</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12">
-        <v>5170.1000000000004</v>
+      <c r="B3" s="12"/>
+      <c r="C3" s="15">
+        <v>827.5</v>
       </c>
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12">
-        <v>1712</v>
+      <c r="B4" s="12"/>
+      <c r="C4" s="10">
+        <v>998.1</v>
       </c>
       <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="13">
-        <v>0.36049999999999915</v>
+      <c r="B5" s="12"/>
+      <c r="C5">
+        <v>0.1177999999999999</v>
       </c>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="14">
-        <v>1.0245470760959214</v>
+      <c r="B6" s="12"/>
+      <c r="C6" s="16">
+        <v>1.0330189803751355</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4">
         <v>60</v>
       </c>
@@ -551,8 +561,8 @@
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="15">
-        <v>52437</v>
+      <c r="C9" s="13">
+        <v>57094.9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -562,8 +572,8 @@
       <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="15">
-        <v>9144.4</v>
+      <c r="C10" s="14">
+        <v>9342.9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,8 +583,8 @@
       <c r="B11" s="5">
         <v>3</v>
       </c>
-      <c r="C11" s="15">
-        <v>2880.5</v>
+      <c r="C11" s="14">
+        <v>3802.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -584,8 +594,8 @@
       <c r="B12" s="6">
         <v>4</v>
       </c>
-      <c r="C12" s="15">
-        <v>1585.1</v>
+      <c r="C12" s="14">
+        <v>2419.1999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,8 +605,8 @@
       <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="15">
-        <v>1156.5</v>
+      <c r="C13" s="14">
+        <v>1858.8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,8 +616,8 @@
       <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="15">
-        <v>923.4</v>
+      <c r="C14" s="14">
+        <v>1358.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,8 +627,8 @@
       <c r="B15" s="5">
         <v>7</v>
       </c>
-      <c r="C15" s="15">
-        <v>788.8</v>
+      <c r="C15" s="14">
+        <v>993.9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,8 +638,8 @@
       <c r="B16" s="5">
         <v>8</v>
       </c>
-      <c r="C16" s="15">
-        <v>720.7</v>
+      <c r="C16" s="14">
+        <v>937.2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,8 +649,8 @@
       <c r="B17" s="5">
         <v>9</v>
       </c>
-      <c r="C17" s="15">
-        <v>764.2</v>
+      <c r="C17" s="14">
+        <v>664.6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,8 +660,8 @@
       <c r="B18" s="6">
         <v>10</v>
       </c>
-      <c r="C18" s="15">
-        <v>649</v>
+      <c r="C18" s="14">
+        <v>570</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,10 +669,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="6">
-        <v>11.5</v>
-      </c>
-      <c r="C19" s="15">
-        <v>644.5</v>
+        <v>12</v>
+      </c>
+      <c r="C19" s="14">
+        <v>774.3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -670,10 +680,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="5">
-        <v>13</v>
-      </c>
-      <c r="C20" s="15">
-        <v>738.4</v>
+        <v>14</v>
+      </c>
+      <c r="C20" s="14">
+        <v>739.6</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,10 +691,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="5">
-        <v>14.5</v>
-      </c>
-      <c r="C21" s="15">
-        <v>549.79999999999995</v>
+        <v>16</v>
+      </c>
+      <c r="C21" s="14">
+        <v>611.79999999999995</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -692,10 +702,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="5">
-        <v>16</v>
-      </c>
-      <c r="C22" s="15">
-        <v>522</v>
+        <v>18</v>
+      </c>
+      <c r="C22" s="14">
+        <v>508.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,10 +713,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="5">
-        <v>17.5</v>
-      </c>
-      <c r="C23" s="15">
-        <v>544</v>
+        <v>20</v>
+      </c>
+      <c r="C23" s="14">
+        <v>482.1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -714,10 +724,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="5">
-        <v>19</v>
-      </c>
-      <c r="C24" s="15">
-        <v>496.6</v>
+        <v>22</v>
+      </c>
+      <c r="C24" s="14">
+        <v>405.7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,10 +735,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="C25" s="15">
-        <v>438.6</v>
+        <v>24</v>
+      </c>
+      <c r="C25" s="14">
+        <v>370.6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,10 +746,10 @@
         <v>18</v>
       </c>
       <c r="B26" s="5">
-        <v>22</v>
-      </c>
-      <c r="C26" s="15">
-        <v>352.3</v>
+        <v>26</v>
+      </c>
+      <c r="C26" s="14">
+        <v>366.4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -747,10 +757,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="5">
-        <v>23.5</v>
-      </c>
-      <c r="C27" s="15">
-        <v>392.9</v>
+        <v>28</v>
+      </c>
+      <c r="C27" s="14">
+        <v>293.2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,10 +768,10 @@
         <v>20</v>
       </c>
       <c r="B28" s="5">
-        <v>25</v>
-      </c>
-      <c r="C28" s="15">
-        <v>297.89999999999998</v>
+        <v>32</v>
+      </c>
+      <c r="C28" s="14">
+        <v>428.6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,10 +779,10 @@
         <v>21</v>
       </c>
       <c r="B29" s="5">
-        <v>27</v>
-      </c>
-      <c r="C29" s="15">
-        <v>472.1</v>
+        <v>36</v>
+      </c>
+      <c r="C29" s="14">
+        <v>463.4</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,99 +790,43 @@
         <v>22</v>
       </c>
       <c r="B30" s="5">
-        <v>29</v>
-      </c>
-      <c r="C30" s="15">
-        <v>382.1</v>
+        <v>40</v>
+      </c>
+      <c r="C30" s="14">
+        <v>279.8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>23</v>
-      </c>
-      <c r="B31" s="5">
-        <v>31</v>
-      </c>
-      <c r="C31" s="15">
-        <v>412.9</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>24</v>
-      </c>
-      <c r="B32" s="5">
-        <v>33</v>
-      </c>
-      <c r="C32" s="15">
-        <v>399.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>25</v>
-      </c>
-      <c r="B33" s="5">
-        <v>35</v>
-      </c>
-      <c r="C33" s="15">
-        <v>322.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>26</v>
-      </c>
-      <c r="B34" s="5">
-        <v>37</v>
-      </c>
-      <c r="C34" s="15">
-        <v>375.2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>27</v>
-      </c>
-      <c r="B35" s="5">
-        <v>39</v>
-      </c>
-      <c r="C35" s="15">
-        <v>342.1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>28</v>
-      </c>
-      <c r="B36" s="5">
-        <v>41</v>
-      </c>
-      <c r="C36" s="15">
-        <v>387.8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>29</v>
-      </c>
-      <c r="B37" s="5">
-        <v>43</v>
-      </c>
-      <c r="C37" s="15">
-        <v>303.89999999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>30</v>
-      </c>
-      <c r="B38" s="5">
-        <v>45</v>
-      </c>
-      <c r="C38" s="15">
-        <v>324.3</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="11"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="11"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="11"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="11"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="11"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
both subj and obj analysis excel sheet output seem to work, even accounting for missing points (due to negative antilog). Excel.py needs refactoring
</commit_message>
<xml_diff>
--- a/CATE Template - Single Run.xlsx
+++ b/CATE Template - Single Run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Vial #</t>
   </si>
@@ -40,7 +40,10 @@
     <t>Load Time (min)</t>
   </si>
   <si>
-    <t>Run5</t>
+    <t>Run1</t>
+  </si>
+  <si>
+    <t>Activity in eluant (cpm)</t>
   </si>
 </sst>
 </file>
@@ -78,7 +81,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,18 +90,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -127,12 +124,40 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -141,7 +166,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -155,20 +180,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,73 +498,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2">
-        <v>7180.7628571428577</v>
-      </c>
-      <c r="D2" s="7"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="5">
+        <v>35714.844999999994</v>
+      </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="15">
-        <v>827.5</v>
-      </c>
-      <c r="D3" s="8"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="6">
+        <v>8679.2999999999993</v>
+      </c>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="10">
-        <v>998.1</v>
-      </c>
-      <c r="D4" s="8"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="6">
+        <v>4746.2</v>
+      </c>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5">
-        <v>0.1177999999999999</v>
-      </c>
-      <c r="D5" s="9"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="7">
+        <v>0.60270000000000046</v>
+      </c>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="16">
-        <v>1.0330189803751355</v>
+      <c r="B6" s="13"/>
+      <c r="C6">
+        <v>1.0084176343828561</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="4">
+      <c r="B7" s="13"/>
+      <c r="C7" s="10">
         <v>60</v>
       </c>
       <c r="D7" s="4"/>
@@ -552,281 +576,340 @@
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C8" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="11">
         <v>1</v>
       </c>
-      <c r="C9" s="13">
-        <v>57094.9</v>
+      <c r="C9" s="8">
+        <v>81453</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="11">
         <v>2</v>
       </c>
-      <c r="C10" s="14">
-        <v>9342.9</v>
+      <c r="C10" s="8">
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="11">
         <v>3</v>
       </c>
-      <c r="C11" s="14">
-        <v>3802.5</v>
+      <c r="C11" s="8">
+        <v>5511</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="11">
         <v>4</v>
       </c>
-      <c r="C12" s="14">
-        <v>2419.1999999999998</v>
+      <c r="C12" s="8">
+        <v>2790.7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="11">
         <v>5</v>
       </c>
-      <c r="C13" s="14">
-        <v>1858.8</v>
+      <c r="C13" s="8">
+        <v>1933.8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="11">
         <v>6</v>
       </c>
-      <c r="C14" s="14">
-        <v>1358.5</v>
+      <c r="C14" s="8">
+        <v>1456.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="11">
         <v>7</v>
       </c>
-      <c r="C15" s="14">
-        <v>993.9</v>
+      <c r="C15" s="8">
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="11">
         <v>8</v>
       </c>
-      <c r="C16" s="14">
-        <v>937.2</v>
+      <c r="C16" s="8">
+        <v>1015.1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="11">
         <v>9</v>
       </c>
-      <c r="C17" s="14">
-        <v>664.6</v>
+      <c r="C17" s="8">
+        <v>882.4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="11">
         <v>10</v>
       </c>
-      <c r="C18" s="14">
-        <v>570</v>
+      <c r="C18" s="8">
+        <v>788.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
-      <c r="B19" s="6">
-        <v>12</v>
-      </c>
-      <c r="C19" s="14">
-        <v>774.3</v>
+      <c r="B19" s="11">
+        <v>11.5</v>
+      </c>
+      <c r="C19" s="8">
+        <v>801.7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
-      <c r="B20" s="5">
-        <v>14</v>
-      </c>
-      <c r="C20" s="14">
-        <v>739.6</v>
+      <c r="B20" s="11">
+        <v>13</v>
+      </c>
+      <c r="C20" s="8">
+        <v>698.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
-      <c r="B21" s="5">
-        <v>16</v>
-      </c>
-      <c r="C21" s="14">
-        <v>611.79999999999995</v>
+      <c r="B21" s="11">
+        <v>14.5</v>
+      </c>
+      <c r="C21" s="8">
+        <v>647.9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
-      <c r="B22" s="5">
-        <v>18</v>
-      </c>
-      <c r="C22" s="14">
-        <v>508.5</v>
+      <c r="B22" s="11">
+        <v>16</v>
+      </c>
+      <c r="C22" s="8">
+        <v>629.29999999999995</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
-      <c r="B23" s="5">
-        <v>20</v>
-      </c>
-      <c r="C23" s="14">
-        <v>482.1</v>
+      <c r="B23" s="11">
+        <v>17.5</v>
+      </c>
+      <c r="C23" s="8">
+        <v>622.20000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
-      <c r="B24" s="5">
-        <v>22</v>
-      </c>
-      <c r="C24" s="14">
-        <v>405.7</v>
+      <c r="B24" s="11">
+        <v>19</v>
+      </c>
+      <c r="C24" s="8">
+        <v>507.9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17</v>
       </c>
-      <c r="B25" s="5">
-        <v>24</v>
-      </c>
-      <c r="C25" s="14">
-        <v>370.6</v>
+      <c r="B25" s="11">
+        <v>20.5</v>
+      </c>
+      <c r="C25" s="8">
+        <v>504.2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
-      <c r="B26" s="5">
-        <v>26</v>
-      </c>
-      <c r="C26" s="14">
-        <v>366.4</v>
+      <c r="B26" s="11">
+        <v>22</v>
+      </c>
+      <c r="C26" s="8">
+        <v>422.8</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
-      <c r="B27" s="5">
-        <v>28</v>
-      </c>
-      <c r="C27" s="14">
-        <v>293.2</v>
+      <c r="B27" s="11">
+        <v>23.5</v>
+      </c>
+      <c r="C27" s="8">
+        <v>451.9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
-      <c r="B28" s="5">
-        <v>32</v>
-      </c>
-      <c r="C28" s="14">
-        <v>428.6</v>
+      <c r="B28" s="11">
+        <v>25</v>
+      </c>
+      <c r="C28" s="8">
+        <v>411.3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
-      <c r="B29" s="5">
-        <v>36</v>
-      </c>
-      <c r="C29" s="14">
-        <v>463.4</v>
+      <c r="B29" s="11">
+        <v>27</v>
+      </c>
+      <c r="C29" s="8">
+        <v>475.7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22</v>
       </c>
-      <c r="B30" s="5">
-        <v>40</v>
-      </c>
-      <c r="C30" s="14">
-        <v>279.8</v>
+      <c r="B30" s="11">
+        <v>29</v>
+      </c>
+      <c r="C30" s="8">
+        <v>453.3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="11"/>
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31" s="11">
+        <v>31</v>
+      </c>
+      <c r="C31" s="8">
+        <v>467.4</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="11"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-      <c r="C37" s="11"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
-      <c r="C38" s="11"/>
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32" s="11">
+        <v>33</v>
+      </c>
+      <c r="C32" s="8">
+        <v>431.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33" s="11">
+        <v>35</v>
+      </c>
+      <c r="C33" s="8">
+        <v>404.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" s="11">
+        <v>37</v>
+      </c>
+      <c r="C34" s="8">
+        <v>432.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35" s="11">
+        <v>39</v>
+      </c>
+      <c r="C35" s="8">
+        <v>363.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36" s="11">
+        <v>41</v>
+      </c>
+      <c r="C36" s="8">
+        <v>429.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>29</v>
+      </c>
+      <c r="B37" s="11">
+        <v>43</v>
+      </c>
+      <c r="C37" s="8">
+        <v>303.39999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38" s="12">
+        <v>45</v>
+      </c>
+      <c r="C38" s="8">
+        <v>348.1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>